<commit_message>
Completed Changing the Background Color of a Cell
</commit_message>
<xml_diff>
--- a/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
+++ b/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/06 - Formatting Data in an Excel Worksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76183BA7-B0C6-4D11-9B5A-233E3CB68E35}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73BECB3C-5FDF-4E44-A2C6-BFD9AE2BFB4F}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,17 +98,23 @@
     <font>
       <b/>
       <sz val="24"/>
-      <color theme="3" tint="0.499984740745262"/>
+      <color theme="0"/>
       <name val="Arial Black"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -123,10 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,7 +471,7 @@
   <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -479,6 +486,11 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">

</xml_diff>

<commit_message>
Completed Adding Borders to Cells
</commit_message>
<xml_diff>
--- a/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
+++ b/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/06 - Formatting Data in an Excel Worksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="107" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73BECB3C-5FDF-4E44-A2C6-BFD9AE2BFB4F}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4906E18-4714-4636-9ACB-54D2E8DB4888}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,12 +117,21 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -132,8 +141,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,7 +491,7 @@
     <col min="8" max="8" width="11.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="37" x14ac:dyDescent="1.05">
+    <row r="2" spans="2:8" ht="37.5" thickBot="1" x14ac:dyDescent="1.1000000000000001">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Completed Excel Cell Borders Continued
</commit_message>
<xml_diff>
--- a/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
+++ b/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/06 - Formatting Data in an Excel Worksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4906E18-4714-4636-9ACB-54D2E8DB4888}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5298C5B4-2E87-4784-BD8A-FED0F963529E}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,7 +117,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -134,15 +134,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFFFC000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,7 +490,7 @@
   <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,39 +502,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="37.5" thickBot="1" x14ac:dyDescent="1.1000000000000001">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>42736</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="4">
         <v>42767</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>42795</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="4">
         <v>42826</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Completed Formatting Data as Currency Values
</commit_message>
<xml_diff>
--- a/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
+++ b/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/06 - Formatting Data in an Excel Worksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5298C5B4-2E87-4784-BD8A-FED0F963529E}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DBCAA0C-E3C2-4ED7-A582-9E965ADB471A}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -84,10 +84,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="mmm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,6 +103,13 @@
       <color theme="0"/>
       <name val="Arial Black"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -144,17 +153,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -490,15 +503,14 @@
   <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.26953125" customWidth="1"/>
     <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="7" width="10.81640625" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" customWidth="1"/>
+    <col min="3" max="8" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="37.5" thickBot="1" x14ac:dyDescent="1.1000000000000001">
@@ -538,19 +550,19 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>1200</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>1200</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="5">
         <v>1000</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="5">
         <v>900</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="5">
         <f t="shared" ref="G5:G11" si="0">SUM(C5:F5)</f>
         <v>4300</v>
       </c>
@@ -563,19 +575,19 @@
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="6">
         <v>100</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <v>135</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="6">
         <v>100</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="6">
         <v>200</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="6">
         <f t="shared" si="0"/>
         <v>535</v>
       </c>
@@ -588,19 +600,19 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="6">
         <v>150</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="6">
         <v>200</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <v>125</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="6">
         <v>150</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="6">
         <f t="shared" si="0"/>
         <v>625</v>
       </c>
@@ -613,19 +625,19 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="6">
         <v>50</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <v>40</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <v>70</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="6">
         <v>30</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="6">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
@@ -638,19 +650,19 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>300</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>275</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>350</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <v>300</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="6">
         <f t="shared" si="0"/>
         <v>1225</v>
       </c>
@@ -663,19 +675,19 @@
       <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>100</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>100</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>110</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <v>150</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="6">
         <f t="shared" si="0"/>
         <v>460</v>
       </c>
@@ -688,23 +700,23 @@
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <f>SUM(C5:C10)</f>
         <v>1900</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <f t="shared" ref="D11:F11" si="2">SUM(D5:D10)</f>
         <v>1950</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="5">
         <f t="shared" si="2"/>
         <v>1755</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="5">
         <f t="shared" si="2"/>
         <v>1730</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>7335</v>
       </c>

</xml_diff>

<commit_message>
Completed Using Excel's Format Painter
</commit_message>
<xml_diff>
--- a/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
+++ b/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/06 - Formatting Data in an Excel Worksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5A4DE9C-503D-4A79-830A-690C3FB111FC}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B6EDA84-1852-41FC-8A33-31CFB85A3850}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Monthly Budget" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -89,7 +89,7 @@
     <numFmt numFmtId="164" formatCode="mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,8 +111,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -122,6 +130,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -158,7 +172,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -167,6 +181,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -506,7 +523,7 @@
   <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -728,8 +745,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
+    <row r="13" spans="2:8" ht="16" x14ac:dyDescent="0.4">
+      <c r="B13" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C13">
@@ -745,8 +762,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+    <row r="14" spans="2:8" ht="16" x14ac:dyDescent="0.4">
+      <c r="B14" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C14">
@@ -762,8 +779,8 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
+    <row r="15" spans="2:8" ht="16" x14ac:dyDescent="0.4">
+      <c r="B15" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C15">
@@ -779,8 +796,8 @@
         <v>292.5</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
+    <row r="16" spans="2:8" ht="16" x14ac:dyDescent="0.4">
+      <c r="B16" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C16">

</xml_diff>

<commit_message>
Completed Creating Styles to Format Data
</commit_message>
<xml_diff>
--- a/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
+++ b/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/06 - Formatting Data in an Excel Worksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B6EDA84-1852-41FC-8A33-31CFB85A3850}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{401FC9B4-F214-4B27-8B2E-48EF8BC660DE}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,7 +120,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +136,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -167,25 +173,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="AwesomeStyle" xfId="3" xr:uid="{494454CA-676D-4A5B-9C23-B38E2E796BC6}"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
@@ -523,7 +531,7 @@
   <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,26 +551,26 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="4" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B4" s="3" t="s">
+    <row r="4" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="8">
         <v>42736</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="8">
         <v>42767</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="8">
         <v>42795</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="8">
         <v>42826</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -570,23 +578,23 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>1200</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <v>1200</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>1000</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <v>900</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <f t="shared" ref="G5:G11" si="0">SUM(C5:F5)</f>
         <v>4300</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="5">
         <f t="shared" ref="H5:H11" si="1">G5/$G$11</f>
         <v>0.58623040218132239</v>
       </c>
@@ -595,23 +603,23 @@
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="4">
         <v>100</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>135</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="4">
         <v>100</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="4">
         <v>200</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>535</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="5">
         <f t="shared" si="1"/>
         <v>7.2937968643490114E-2</v>
       </c>
@@ -620,23 +628,23 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="4">
         <v>150</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="4">
         <v>200</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="4">
         <v>125</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="4">
         <v>150</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>625</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="5">
         <f t="shared" si="1"/>
         <v>8.5207907293796861E-2</v>
       </c>
@@ -645,23 +653,23 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="4">
         <v>50</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <v>40</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="4">
         <v>70</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="4">
         <v>30</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="5">
         <f t="shared" si="1"/>
         <v>2.5903203817314247E-2</v>
       </c>
@@ -670,23 +678,23 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="4">
         <v>300</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="4">
         <v>275</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="4">
         <v>350</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="4">
         <v>300</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
         <v>1225</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="5">
         <f t="shared" si="1"/>
         <v>0.16700749829584186</v>
       </c>
@@ -695,23 +703,23 @@
       <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="4">
         <v>100</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="4">
         <v>100</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="4">
         <v>110</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="4">
         <v>150</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>460</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="5">
         <f t="shared" si="1"/>
         <v>6.2713019768234499E-2</v>
       </c>
@@ -720,33 +728,33 @@
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <f>SUM(C5:C10)</f>
         <v>1900</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <f t="shared" ref="D11:F11" si="2">SUM(D5:D10)</f>
         <v>1950</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <f t="shared" si="2"/>
         <v>1755</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
         <f t="shared" si="2"/>
         <v>1730</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>7335</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="5">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="16" x14ac:dyDescent="0.4">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C13">
@@ -763,7 +771,7 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="16" x14ac:dyDescent="0.4">
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C14">
@@ -780,7 +788,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="16" x14ac:dyDescent="0.4">
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C15">
@@ -797,7 +805,7 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="16" x14ac:dyDescent="0.4">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C16">

</xml_diff>

<commit_message>
Completed Merging and Centering Cells
</commit_message>
<xml_diff>
--- a/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
+++ b/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/06 - Formatting Data in an Excel Worksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{401FC9B4-F214-4B27-8B2E-48EF8BC660DE}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53B923BE-4BDE-4F4A-9DA8-FEE53D9DE448}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -146,21 +146,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -177,20 +168,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3"/>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="2" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="AwesomeStyle" xfId="3" xr:uid="{494454CA-676D-4A5B-9C23-B38E2E796BC6}"/>
@@ -531,7 +523,7 @@
   <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,36 +533,37 @@
     <col min="3" max="8" width="13.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="37.5" thickBot="1" x14ac:dyDescent="1.1000000000000001">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:8" ht="37" x14ac:dyDescent="1.05">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="4" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>42736</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>42767</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>42795</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <v>42826</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -578,23 +571,23 @@
       <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="1">
         <v>1200</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>1200</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="1">
         <v>1000</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <v>900</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="1">
         <f t="shared" ref="G5:G11" si="0">SUM(C5:F5)</f>
         <v>4300</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <f t="shared" ref="H5:H11" si="1">G5/$G$11</f>
         <v>0.58623040218132239</v>
       </c>
@@ -603,23 +596,23 @@
       <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <v>100</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>135</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <v>100</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>200</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="2">
         <f t="shared" si="0"/>
         <v>535</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <f t="shared" si="1"/>
         <v>7.2937968643490114E-2</v>
       </c>
@@ -628,23 +621,23 @@
       <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <v>150</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>200</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <v>125</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="2">
         <v>150</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="2">
         <f t="shared" si="0"/>
         <v>625</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <f t="shared" si="1"/>
         <v>8.5207907293796861E-2</v>
       </c>
@@ -653,23 +646,23 @@
       <c r="B8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <v>50</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <v>40</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
         <v>70</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="2">
         <v>30</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>190</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="3">
         <f t="shared" si="1"/>
         <v>2.5903203817314247E-2</v>
       </c>
@@ -678,23 +671,23 @@
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="2">
         <v>300</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2">
         <v>275</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="2">
         <v>350</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="2">
         <v>300</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="2">
         <f t="shared" si="0"/>
         <v>1225</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="3">
         <f t="shared" si="1"/>
         <v>0.16700749829584186</v>
       </c>
@@ -703,23 +696,23 @@
       <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="2">
         <v>100</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="2">
         <v>100</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="2">
         <v>110</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="2">
         <v>150</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="2">
         <f t="shared" si="0"/>
         <v>460</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="3">
         <f t="shared" si="1"/>
         <v>6.2713019768234499E-2</v>
       </c>
@@ -728,33 +721,33 @@
       <c r="B11" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="1">
         <f>SUM(C5:C10)</f>
         <v>1900</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="1">
         <f t="shared" ref="D11:F11" si="2">SUM(D5:D10)</f>
         <v>1950</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="1">
         <f t="shared" si="2"/>
         <v>1755</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="1">
         <f t="shared" si="2"/>
         <v>1730</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="1">
         <f t="shared" si="0"/>
         <v>7335</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="16" x14ac:dyDescent="0.4">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C13">
@@ -771,7 +764,7 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="16" x14ac:dyDescent="0.4">
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C14">
@@ -788,7 +781,7 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="16" x14ac:dyDescent="0.4">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C15">
@@ -805,7 +798,7 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="16" x14ac:dyDescent="0.4">
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C16">
@@ -822,6 +815,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="C13:E16 C11:F11" formulaRange="1"/>

</xml_diff>

<commit_message>
Completed Using Conditional Formatting
</commit_message>
<xml_diff>
--- a/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
+++ b/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/06 - Formatting Data in an Excel Worksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53B923BE-4BDE-4F4A-9DA8-FEE53D9DE448}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A86DF67-C4EA-489C-8BE8-C38392EDB408}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,7 +180,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -190,7 +190,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -522,8 +530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -589,7 +597,7 @@
       </c>
       <c r="H5" s="3">
         <f t="shared" ref="H5:H11" si="1">G5/$G$11</f>
-        <v>0.58623040218132239</v>
+        <v>0.59433310297166553</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
@@ -614,7 +622,7 @@
       </c>
       <c r="H6" s="3">
         <f t="shared" si="1"/>
-        <v>7.2937968643490114E-2</v>
+        <v>7.3946095369730472E-2</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
@@ -639,7 +647,7 @@
       </c>
       <c r="H7" s="3">
         <f t="shared" si="1"/>
-        <v>8.5207907293796861E-2</v>
+        <v>8.6385625431928126E-2</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
@@ -664,7 +672,7 @@
       </c>
       <c r="H8" s="3">
         <f t="shared" si="1"/>
-        <v>2.5903203817314247E-2</v>
+        <v>2.626123013130615E-2</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.35">
@@ -672,7 +680,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="2">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D9" s="2">
         <v>275</v>
@@ -685,11 +693,11 @@
       </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>1225</v>
+        <v>1125</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="1"/>
-        <v>0.16700749829584186</v>
+        <v>0.15549412577747063</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.35">
@@ -714,7 +722,7 @@
       </c>
       <c r="H10" s="3">
         <f t="shared" si="1"/>
-        <v>6.2713019768234499E-2</v>
+        <v>6.3579820317899105E-2</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.35">
@@ -723,7 +731,7 @@
       </c>
       <c r="C11" s="1">
         <f>SUM(C5:C10)</f>
-        <v>1900</v>
+        <v>1800</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" ref="D11:F11" si="2">SUM(D5:D10)</f>
@@ -739,7 +747,7 @@
       </c>
       <c r="G11" s="1">
         <f t="shared" si="0"/>
-        <v>7335</v>
+        <v>7235</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="1"/>
@@ -786,7 +794,7 @@
       </c>
       <c r="C15">
         <f>AVERAGE(C5:C10)</f>
-        <v>316.66666666666669</v>
+        <v>300</v>
       </c>
       <c r="D15">
         <f t="shared" ref="D15:E15" si="5">AVERAGE(D5:D10)</f>
@@ -818,6 +826,11 @@
   <mergeCells count="1">
     <mergeCell ref="B2:H2"/>
   </mergeCells>
+  <conditionalFormatting sqref="C5:F10">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>250</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="C13:E16 C11:F11" formulaRange="1"/>

</xml_diff>

<commit_message>
Completed Editing Excel Conditional Formatting
</commit_message>
<xml_diff>
--- a/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
+++ b/06 - Formatting Data in an Excel Worksheet/MonthlyBudget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/06 - Formatting Data in an Excel Worksheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A86DF67-C4EA-489C-8BE8-C38392EDB408}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="11_AD4DB114E441178AC67DF4EBB612E572693EDF1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6081524E-D8D9-4C2A-AB68-781F6E4EE0FA}"/>
   <bookViews>
     <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,11 +190,18 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -531,7 +538,7 @@
   <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -827,7 +834,7 @@
     <mergeCell ref="B2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:F10">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>250</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>